<commit_message>
coding is freakin fun
</commit_message>
<xml_diff>
--- a/doc/updated Data Dictionary.xlsx
+++ b/doc/updated Data Dictionary.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RuoxiDu/Dropbox/CS4400database/project/part4/parts/updated_prior_work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Desktop/db_2017_airbib/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="2640" windowWidth="28620" windowHeight="15360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
   <si>
     <t>DATA ITEM</t>
   </si>
@@ -131,24 +134,15 @@
     <t>account number of hosts' bank for receiving payment</t>
   </si>
   <si>
-    <t>House</t>
-  </si>
-  <si>
     <t>houseID</t>
   </si>
   <si>
     <t>uniquely identifies house</t>
   </si>
   <si>
-    <t>houseAddress</t>
-  </si>
-  <si>
     <t>address of the house</t>
   </si>
   <si>
-    <t>houseRate</t>
-  </si>
-  <si>
     <t>rate(cost) of staying in the house</t>
   </si>
   <si>
@@ -327,13 +321,34 @@
   </si>
   <si>
     <t>receives</t>
+  </si>
+  <si>
+    <t>Homes</t>
+  </si>
+  <si>
+    <t>homeID</t>
+  </si>
+  <si>
+    <t>homeAddress</t>
+  </si>
+  <si>
+    <t>homeRate</t>
+  </si>
+  <si>
+    <t>decimal(10,2)</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>home_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -345,6 +360,18 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -372,10 +399,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -386,8 +417,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -707,8 +743,8 @@
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+      <c r="C3" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -724,7 +760,9 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
@@ -734,9 +772,11 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -746,9 +786,11 @@
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
@@ -758,7 +800,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -776,7 +818,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -792,16 +834,13 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -812,43 +851,49 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -870,10 +915,10 @@
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -884,10 +929,10 @@
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -898,10 +943,10 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
@@ -912,10 +957,10 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -926,10 +971,10 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
@@ -940,10 +985,10 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -954,10 +999,10 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -968,7 +1013,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -976,10 +1021,10 @@
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -990,10 +1035,10 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -1002,10 +1047,10 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>4</v>
@@ -1014,10 +1059,10 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
@@ -1026,7 +1071,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1034,10 +1079,10 @@
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1048,10 +1093,10 @@
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1059,10 +1104,10 @@
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -1070,10 +1115,10 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>9</v>
@@ -1082,10 +1127,10 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>7</v>
@@ -1096,10 +1141,10 @@
     </row>
     <row r="35" spans="1:4" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -1107,10 +1152,10 @@
     </row>
     <row r="36" spans="1:4" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>13</v>
@@ -1121,7 +1166,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>7</v>
@@ -1132,7 +1177,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1140,10 +1185,10 @@
     </row>
     <row r="39" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -1154,10 +1199,10 @@
     </row>
     <row r="40" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -1166,10 +1211,10 @@
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>6</v>
@@ -1178,7 +1223,7 @@
     </row>
     <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1186,10 +1231,10 @@
     </row>
     <row r="43" spans="1:4" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1200,10 +1245,10 @@
     </row>
     <row r="44" spans="1:4" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>6</v>
@@ -1236,7 +1281,7 @@
     </row>
     <row r="47" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>20</v>
@@ -1248,7 +1293,7 @@
     </row>
     <row r="48" spans="1:4" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1256,10 +1301,10 @@
     </row>
     <row r="49" spans="1:4" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>4</v>
@@ -1284,10 +1329,10 @@
     </row>
     <row r="51" spans="1:4" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>4</v>
@@ -1298,7 +1343,7 @@
     </row>
     <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -1320,10 +1365,10 @@
     </row>
     <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>4</v>
@@ -1334,7 +1379,7 @@
     </row>
     <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -1342,10 +1387,10 @@
     </row>
     <row r="56" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>4</v>
@@ -1370,7 +1415,7 @@
     </row>
     <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -1378,10 +1423,10 @@
     </row>
     <row r="59" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>4</v>
@@ -1406,10 +1451,10 @@
     </row>
     <row r="61" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>4</v>
@@ -1420,7 +1465,7 @@
     </row>
     <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -1428,10 +1473,10 @@
     </row>
     <row r="63" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>4</v>
@@ -1442,10 +1487,10 @@
     </row>
     <row r="64" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>4</v>
@@ -1456,17 +1501,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>